<commit_message>
SAMD21 PWM final implementation
-finished SAMD21 PWM implementation for TC timers
-updated xls map generation file
-added coolant enabled by default (grbl compliant)
</commit_message>
<xml_diff>
--- a/docs/mcumap_gen.xlsx
+++ b/docs/mcumap_gen.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JCEM\Documents\GitHub\uCNC\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5869AE4B-86B8-4CC6-AA11-E8CF80A3BF3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39883AC8-B33C-460A-8228-5CA2280E5D0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="2970" yWindow="3060" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AVR" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,15 @@
     <sheet name="SAMD21" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -941,7 +950,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M996"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+    <sheetView topLeftCell="A94" workbookViewId="0">
       <selection activeCell="F55" sqref="F55"/>
     </sheetView>
   </sheetViews>
@@ -21814,7 +21823,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98F2B596-2266-4C9E-803A-E01078017355}">
   <dimension ref="A1:I996"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
       <selection activeCell="I55" sqref="I55"/>
     </sheetView>
   </sheetViews>
@@ -37958,8 +37967,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A55A102-54D4-49D0-A939-D97717A30533}">
   <dimension ref="A1:M998"/>
   <sheetViews>
-    <sheetView topLeftCell="A90" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3:I104"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23:H38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -39073,61 +39082,109 @@
       <c r="F23" s="6"/>
       <c r="G23" s="6"/>
       <c r="H23" s="6" t="str">
-        <f t="shared" ref="H23:H38" si="4">"#if (defined("&amp;C23&amp;"_OCR) &amp;&amp; defined("&amp;C23&amp;"_TIMER) &amp;&amp; defined("&amp;C23&amp;"))
-#define "&amp;C23&amp;"_OCRREG (__ocrreg__("&amp;C23&amp;"_TIMER, "&amp;C23&amp;"_OCR))
-#define "&amp;C23&amp;"_TMRAREG (__tmrareg__("&amp;C23&amp;"_TIMER))
-#define "&amp;C23&amp;"_TMRBREG (__tmrbreg__("&amp;C23&amp;"_TIMER))
-#define "&amp;C23&amp;"_ENABLE_MASK __pwmenmask__("&amp;C23&amp;"_OCR)
-#if ("&amp;C23&amp;"_TIMER == 2)
-#define "&amp;C23&amp;"_PRESCALLER 0x04
-#elif ("&amp;C23&amp;"_TIMER == 0)
-#define "&amp;C23&amp;"_PRESCALLER 0x03
+        <f>"#ifdef "&amp;C23&amp;"
+#define "&amp;C23&amp;"_CLKCTRL gclk_clkctrl("&amp;C23&amp;"_TIMER)
+#define "&amp;C23&amp;"_PMUX (pinmux("&amp;C23&amp;"_PORT, "&amp;C23&amp;"_BIT))
+#define "&amp;C23&amp;"_PMUXVAL (pinmuxval("&amp;C23&amp;"_MUX))
+#if ("&amp;C23&amp;"_TIMER &lt; 3)
+#define "&amp;C23&amp;"_TMR __helper__(TCC, "&amp;C23&amp;"_TIMER, )
+#define "&amp;C23&amp;"_CONFIG (                         \
+	{                                         \
+		"&amp;C23&amp;"_TMR-&gt;CTRLA.bit.SWRST = 1;        \
+		while ("&amp;C23&amp;"_TMR-&gt;SYNCBUSY.bit.SWRST)  \
+			;                                 \
+		"&amp;C23&amp;"_TMR-&gt;CTRLA.bit.PRESCALER = 7;    \
+		"&amp;C23&amp;"_TMR-&gt;WAVE.bit.WAVEGEN = 2;       \
+		while ("&amp;C23&amp;"_TMR-&gt;SYNCBUSY.bit.WAVE)   \
+			;                                 \
+		"&amp;C23&amp;"_TMR-&gt;PER.bit.PER = 255;          \
+		while ("&amp;C23&amp;"_TMR-&gt;SYNCBUSY.bit.PER)    \
+			;                                 \
+		"&amp;C23&amp;"_TMR-&gt;CTRLA.bit.ENABLE = 1;       \
+		while ("&amp;C23&amp;"_TMR-&gt;SYNCBUSY.bit.ENABLE) \
+			;                                 \
+	})
+#define "&amp;C23&amp;"_DUTYCYCLE ("&amp;C23&amp;"_TMR-&gt;CC["&amp;C23&amp;"_CHANNEL].bit.CC)
 #else
-#define "&amp;C23&amp;"_PRESCALLER 0x0B
-#endif
-#if ("&amp;C23&amp;"_TIMER == 0 || "&amp;C23&amp;"_TIMER == 2)
-#define "&amp;C23&amp;"_MODE 0x03
+#define "&amp;C23&amp;"_TMR __helper__(TC, "&amp;C23&amp;"_TIMER, )
+#define "&amp;C23&amp;"_CONFIG (                                \
+	{                                                \
+		"&amp;C23&amp;"_TMR-&gt;COUNT8.CTRLA.bit.SWRST = 1;        \
+		while ("&amp;C23&amp;"_TMR-&gt;COUNT8.STATUS.bit.SYNCBUSY) \
+			;                                        \
+		"&amp;C23&amp;"_TMR-&gt;COUNT8.CTRLA.bit.MODE = 1;         \
+		"&amp;C23&amp;"_TMR-&gt;COUNT8.CTRLA.bit.PRESCALER = 7;    \
+		"&amp;C23&amp;"_TMR-&gt;COUNT8.CTRLA.bit.WAVEGEN = 2;      \
+		while ("&amp;C23&amp;"_TMR-&gt;COUNT8.STATUS.bit.SYNCBUSY) \
+			;                                        \
+		"&amp;C23&amp;"_TMR-&gt;COUNT8.PER.reg = 255;              \
+		while ("&amp;C23&amp;"_TMR-&gt;COUNT8.STATUS.bit.SYNCBUSY) \
+			;                                        \
+		"&amp;C23&amp;"_TMR-&gt;COUNT8.CTRLA.bit.ENABLE = 1;       \
+		while ("&amp;C23&amp;"_TMR-&gt;COUNT8.STATUS.bit.SYNCBUSY) \
+			;                                        \
+	})
+#define "&amp;C23&amp;"_DUTYCYCLE ("&amp;C23&amp;"_TMR-&gt;COUNT8.CC["&amp;C23&amp;"_CHANNEL].reg)
+#endif
+#define "&amp;B23&amp;"_PMUX "&amp;C23&amp;"_PMUX
+#define "&amp;B23&amp;"_PMUXVAL "&amp;C23&amp;"_PMUXVAL
+#define "&amp;B23&amp;"_TMR "&amp;C23&amp;"_TMR
+#define "&amp;B23&amp;"_CONFIG "&amp;C23&amp;"_CONFIG
+#define "&amp;B23&amp;"_DUTYCYCLE "&amp;C23&amp;"_DUTYCYCLE
+#endif"</f>
+        <v>#ifdef PWM0
+#define PWM0_CLKCTRL gclk_clkctrl(PWM0_TIMER)
+#define PWM0_PMUX (pinmux(PWM0_PORT, PWM0_BIT))
+#define PWM0_PMUXVAL (pinmuxval(PWM0_MUX))
+#if (PWM0_TIMER &lt; 3)
+#define PWM0_TMR __helper__(TCC, PWM0_TIMER, )
+#define PWM0_CONFIG (                         \
+	{                                         \
+		PWM0_TMR-&gt;CTRLA.bit.SWRST = 1;        \
+		while (PWM0_TMR-&gt;SYNCBUSY.bit.SWRST)  \
+			;                                 \
+		PWM0_TMR-&gt;CTRLA.bit.PRESCALER = 7;    \
+		PWM0_TMR-&gt;WAVE.bit.WAVEGEN = 2;       \
+		while (PWM0_TMR-&gt;SYNCBUSY.bit.WAVE)   \
+			;                                 \
+		PWM0_TMR-&gt;PER.bit.PER = 255;          \
+		while (PWM0_TMR-&gt;SYNCBUSY.bit.PER)    \
+			;                                 \
+		PWM0_TMR-&gt;CTRLA.bit.ENABLE = 1;       \
+		while (PWM0_TMR-&gt;SYNCBUSY.bit.ENABLE) \
+			;                                 \
+	})
+#define PWM0_DUTYCYCLE (PWM0_TMR-&gt;CC[PWM0_CHANNEL].bit.CC)
 #else
-#define "&amp;C23&amp;"_MODE 0x01
-#endif
-#define "&amp;B23&amp;"_OCR "&amp;C23&amp;"_OCR
-#define "&amp;B23&amp;"_TIMER "&amp;C23&amp;"_TIMER
-#define "&amp;B23&amp;"_OCRREG "&amp;C23&amp;"_OCRREG
-#define "&amp;B23&amp;"_TMRAREG "&amp;C23&amp;"_TMRAREG
-#define "&amp;B23&amp;"_TMRBREG "&amp;C23&amp;"_TMRBREG
-#define "&amp;B23&amp;"_ENABLE_MASK "&amp;C23&amp;"_ENABLE_MASK
-#define "&amp;B23&amp;"_MODE "&amp;C23&amp;"_MODE
-#define "&amp;B23&amp;"_PRESCALLER "&amp;C23&amp;"_PRESCALLER
-#endif"</f>
-        <v>#if (defined(PWM0_OCR) &amp;&amp; defined(PWM0_TIMER) &amp;&amp; defined(PWM0))
-#define PWM0_OCRREG (__ocrreg__(PWM0_TIMER, PWM0_OCR))
-#define PWM0_TMRAREG (__tmrareg__(PWM0_TIMER))
-#define PWM0_TMRBREG (__tmrbreg__(PWM0_TIMER))
-#define PWM0_ENABLE_MASK __pwmenmask__(PWM0_OCR)
-#if (PWM0_TIMER == 2)
-#define PWM0_PRESCALLER 0x04
-#elif (PWM0_TIMER == 0)
-#define PWM0_PRESCALLER 0x03
-#else
-#define PWM0_PRESCALLER 0x0B
-#endif
-#if (PWM0_TIMER == 0 || PWM0_TIMER == 2)
-#define PWM0_MODE 0x03
-#else
-#define PWM0_MODE 0x01
-#endif
-#define DIO20_OCR PWM0_OCR
-#define DIO20_TIMER PWM0_TIMER
-#define DIO20_OCRREG PWM0_OCRREG
-#define DIO20_TMRAREG PWM0_TMRAREG
-#define DIO20_TMRBREG PWM0_TMRBREG
-#define DIO20_ENABLE_MASK PWM0_ENABLE_MASK
-#define DIO20_MODE PWM0_MODE
-#define DIO20_PRESCALLER PWM0_PRESCALLER
+#define PWM0_TMR __helper__(TC, PWM0_TIMER, )
+#define PWM0_CONFIG (                                \
+	{                                                \
+		PWM0_TMR-&gt;COUNT8.CTRLA.bit.SWRST = 1;        \
+		while (PWM0_TMR-&gt;COUNT8.STATUS.bit.SYNCBUSY) \
+			;                                        \
+		PWM0_TMR-&gt;COUNT8.CTRLA.bit.MODE = 1;         \
+		PWM0_TMR-&gt;COUNT8.CTRLA.bit.PRESCALER = 7;    \
+		PWM0_TMR-&gt;COUNT8.CTRLA.bit.WAVEGEN = 2;      \
+		while (PWM0_TMR-&gt;COUNT8.STATUS.bit.SYNCBUSY) \
+			;                                        \
+		PWM0_TMR-&gt;COUNT8.PER.reg = 255;              \
+		while (PWM0_TMR-&gt;COUNT8.STATUS.bit.SYNCBUSY) \
+			;                                        \
+		PWM0_TMR-&gt;COUNT8.CTRLA.bit.ENABLE = 1;       \
+		while (PWM0_TMR-&gt;COUNT8.STATUS.bit.SYNCBUSY) \
+			;                                        \
+	})
+#define PWM0_DUTYCYCLE (PWM0_TMR-&gt;COUNT8.CC[PWM0_CHANNEL].reg)
+#endif
+#define DIO20_PMUX PWM0_PMUX
+#define DIO20_PMUXVAL PWM0_PMUXVAL
+#define DIO20_TMR PWM0_TMR
+#define DIO20_CONFIG PWM0_CONFIG
+#define DIO20_DUTYCYCLE PWM0_DUTYCYCLE
 #endif</v>
       </c>
       <c r="I23" s="3" t="str">
-        <f t="shared" ref="I23:I38" si="5">"#ifdef "&amp;C23&amp;"
+        <f t="shared" ref="I23:I38" si="4">"#ifdef "&amp;C23&amp;"
 mcu_config_pwm("&amp;C23&amp;");
 #endif"</f>
         <v>#ifdef PWM0
@@ -39167,36 +39224,109 @@
       <c r="F24" s="6"/>
       <c r="G24" s="6"/>
       <c r="H24" s="6" t="str">
+        <f t="shared" ref="H24:H38" si="5">"#ifdef "&amp;C24&amp;"
+#define "&amp;C24&amp;"_CLKCTRL gclk_clkctrl("&amp;C24&amp;"_TIMER)
+#define "&amp;C24&amp;"_PMUX (pinmux("&amp;C24&amp;"_PORT, "&amp;C24&amp;"_BIT))
+#define "&amp;C24&amp;"_PMUXVAL (pinmuxval("&amp;C24&amp;"_MUX))
+#if ("&amp;C24&amp;"_TIMER &lt; 3)
+#define "&amp;C24&amp;"_TMR __helper__(TCC, "&amp;C24&amp;"_TIMER, )
+#define "&amp;C24&amp;"_CONFIG (                         \
+	{                                         \
+		"&amp;C24&amp;"_TMR-&gt;CTRLA.bit.SWRST = 1;        \
+		while ("&amp;C24&amp;"_TMR-&gt;SYNCBUSY.bit.SWRST)  \
+			;                                 \
+		"&amp;C24&amp;"_TMR-&gt;CTRLA.bit.PRESCALER = 7;    \
+		"&amp;C24&amp;"_TMR-&gt;WAVE.bit.WAVEGEN = 2;       \
+		while ("&amp;C24&amp;"_TMR-&gt;SYNCBUSY.bit.WAVE)   \
+			;                                 \
+		"&amp;C24&amp;"_TMR-&gt;PER.bit.PER = 255;          \
+		while ("&amp;C24&amp;"_TMR-&gt;SYNCBUSY.bit.PER)    \
+			;                                 \
+		"&amp;C24&amp;"_TMR-&gt;CTRLA.bit.ENABLE = 1;       \
+		while ("&amp;C24&amp;"_TMR-&gt;SYNCBUSY.bit.ENABLE) \
+			;                                 \
+	})
+#define "&amp;C24&amp;"_DUTYCYCLE ("&amp;C24&amp;"_TMR-&gt;CC["&amp;C24&amp;"_CHANNEL].bit.CC)
+#else
+#define "&amp;C24&amp;"_TMR __helper__(TC, "&amp;C24&amp;"_TIMER, )
+#define "&amp;C24&amp;"_CONFIG (                                \
+	{                                                \
+		"&amp;C24&amp;"_TMR-&gt;COUNT8.CTRLA.bit.SWRST = 1;        \
+		while ("&amp;C24&amp;"_TMR-&gt;COUNT8.STATUS.bit.SYNCBUSY) \
+			;                                        \
+		"&amp;C24&amp;"_TMR-&gt;COUNT8.CTRLA.bit.MODE = 1;         \
+		"&amp;C24&amp;"_TMR-&gt;COUNT8.CTRLA.bit.PRESCALER = 7;    \
+		"&amp;C24&amp;"_TMR-&gt;COUNT8.CTRLA.bit.WAVEGEN = 2;      \
+		while ("&amp;C24&amp;"_TMR-&gt;COUNT8.STATUS.bit.SYNCBUSY) \
+			;                                        \
+		"&amp;C24&amp;"_TMR-&gt;COUNT8.PER.reg = 255;              \
+		while ("&amp;C24&amp;"_TMR-&gt;COUNT8.STATUS.bit.SYNCBUSY) \
+			;                                        \
+		"&amp;C24&amp;"_TMR-&gt;COUNT8.CTRLA.bit.ENABLE = 1;       \
+		while ("&amp;C24&amp;"_TMR-&gt;COUNT8.STATUS.bit.SYNCBUSY) \
+			;                                        \
+	})
+#define "&amp;C24&amp;"_DUTYCYCLE ("&amp;C24&amp;"_TMR-&gt;COUNT8.CC["&amp;C24&amp;"_CHANNEL].reg)
+#endif
+#define "&amp;B24&amp;"_PMUX "&amp;C24&amp;"_PMUX
+#define "&amp;B24&amp;"_PMUXVAL "&amp;C24&amp;"_PMUXVAL
+#define "&amp;B24&amp;"_TMR "&amp;C24&amp;"_TMR
+#define "&amp;B24&amp;"_CONFIG "&amp;C24&amp;"_CONFIG
+#define "&amp;B24&amp;"_DUTYCYCLE "&amp;C24&amp;"_DUTYCYCLE
+#endif"</f>
+        <v>#ifdef PWM1
+#define PWM1_CLKCTRL gclk_clkctrl(PWM1_TIMER)
+#define PWM1_PMUX (pinmux(PWM1_PORT, PWM1_BIT))
+#define PWM1_PMUXVAL (pinmuxval(PWM1_MUX))
+#if (PWM1_TIMER &lt; 3)
+#define PWM1_TMR __helper__(TCC, PWM1_TIMER, )
+#define PWM1_CONFIG (                         \
+	{                                         \
+		PWM1_TMR-&gt;CTRLA.bit.SWRST = 1;        \
+		while (PWM1_TMR-&gt;SYNCBUSY.bit.SWRST)  \
+			;                                 \
+		PWM1_TMR-&gt;CTRLA.bit.PRESCALER = 7;    \
+		PWM1_TMR-&gt;WAVE.bit.WAVEGEN = 2;       \
+		while (PWM1_TMR-&gt;SYNCBUSY.bit.WAVE)   \
+			;                                 \
+		PWM1_TMR-&gt;PER.bit.PER = 255;          \
+		while (PWM1_TMR-&gt;SYNCBUSY.bit.PER)    \
+			;                                 \
+		PWM1_TMR-&gt;CTRLA.bit.ENABLE = 1;       \
+		while (PWM1_TMR-&gt;SYNCBUSY.bit.ENABLE) \
+			;                                 \
+	})
+#define PWM1_DUTYCYCLE (PWM1_TMR-&gt;CC[PWM1_CHANNEL].bit.CC)
+#else
+#define PWM1_TMR __helper__(TC, PWM1_TIMER, )
+#define PWM1_CONFIG (                                \
+	{                                                \
+		PWM1_TMR-&gt;COUNT8.CTRLA.bit.SWRST = 1;        \
+		while (PWM1_TMR-&gt;COUNT8.STATUS.bit.SYNCBUSY) \
+			;                                        \
+		PWM1_TMR-&gt;COUNT8.CTRLA.bit.MODE = 1;         \
+		PWM1_TMR-&gt;COUNT8.CTRLA.bit.PRESCALER = 7;    \
+		PWM1_TMR-&gt;COUNT8.CTRLA.bit.WAVEGEN = 2;      \
+		while (PWM1_TMR-&gt;COUNT8.STATUS.bit.SYNCBUSY) \
+			;                                        \
+		PWM1_TMR-&gt;COUNT8.PER.reg = 255;              \
+		while (PWM1_TMR-&gt;COUNT8.STATUS.bit.SYNCBUSY) \
+			;                                        \
+		PWM1_TMR-&gt;COUNT8.CTRLA.bit.ENABLE = 1;       \
+		while (PWM1_TMR-&gt;COUNT8.STATUS.bit.SYNCBUSY) \
+			;                                        \
+	})
+#define PWM1_DUTYCYCLE (PWM1_TMR-&gt;COUNT8.CC[PWM1_CHANNEL].reg)
+#endif
+#define DIO21_PMUX PWM1_PMUX
+#define DIO21_PMUXVAL PWM1_PMUXVAL
+#define DIO21_TMR PWM1_TMR
+#define DIO21_CONFIG PWM1_CONFIG
+#define DIO21_DUTYCYCLE PWM1_DUTYCYCLE
+#endif</v>
+      </c>
+      <c r="I24" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>#if (defined(PWM1_OCR) &amp;&amp; defined(PWM1_TIMER) &amp;&amp; defined(PWM1))
-#define PWM1_OCRREG (__ocrreg__(PWM1_TIMER, PWM1_OCR))
-#define PWM1_TMRAREG (__tmrareg__(PWM1_TIMER))
-#define PWM1_TMRBREG (__tmrbreg__(PWM1_TIMER))
-#define PWM1_ENABLE_MASK __pwmenmask__(PWM1_OCR)
-#if (PWM1_TIMER == 2)
-#define PWM1_PRESCALLER 0x04
-#elif (PWM1_TIMER == 0)
-#define PWM1_PRESCALLER 0x03
-#else
-#define PWM1_PRESCALLER 0x0B
-#endif
-#if (PWM1_TIMER == 0 || PWM1_TIMER == 2)
-#define PWM1_MODE 0x03
-#else
-#define PWM1_MODE 0x01
-#endif
-#define DIO21_OCR PWM1_OCR
-#define DIO21_TIMER PWM1_TIMER
-#define DIO21_OCRREG PWM1_OCRREG
-#define DIO21_TMRAREG PWM1_TMRAREG
-#define DIO21_TMRBREG PWM1_TMRBREG
-#define DIO21_ENABLE_MASK PWM1_ENABLE_MASK
-#define DIO21_MODE PWM1_MODE
-#define DIO21_PRESCALLER PWM1_PRESCALLER
-#endif</v>
-      </c>
-      <c r="I24" s="3" t="str">
-        <f t="shared" si="5"/>
         <v>#ifdef PWM1
 mcu_config_pwm(PWM1);
 #endif</v>
@@ -39234,36 +39364,60 @@
       <c r="F25" s="6"/>
       <c r="G25" s="6"/>
       <c r="H25" s="6" t="str">
+        <f t="shared" si="5"/>
+        <v>#ifdef PWM2
+#define PWM2_CLKCTRL gclk_clkctrl(PWM2_TIMER)
+#define PWM2_PMUX (pinmux(PWM2_PORT, PWM2_BIT))
+#define PWM2_PMUXVAL (pinmuxval(PWM2_MUX))
+#if (PWM2_TIMER &lt; 3)
+#define PWM2_TMR __helper__(TCC, PWM2_TIMER, )
+#define PWM2_CONFIG (                         \
+	{                                         \
+		PWM2_TMR-&gt;CTRLA.bit.SWRST = 1;        \
+		while (PWM2_TMR-&gt;SYNCBUSY.bit.SWRST)  \
+			;                                 \
+		PWM2_TMR-&gt;CTRLA.bit.PRESCALER = 7;    \
+		PWM2_TMR-&gt;WAVE.bit.WAVEGEN = 2;       \
+		while (PWM2_TMR-&gt;SYNCBUSY.bit.WAVE)   \
+			;                                 \
+		PWM2_TMR-&gt;PER.bit.PER = 255;          \
+		while (PWM2_TMR-&gt;SYNCBUSY.bit.PER)    \
+			;                                 \
+		PWM2_TMR-&gt;CTRLA.bit.ENABLE = 1;       \
+		while (PWM2_TMR-&gt;SYNCBUSY.bit.ENABLE) \
+			;                                 \
+	})
+#define PWM2_DUTYCYCLE (PWM2_TMR-&gt;CC[PWM2_CHANNEL].bit.CC)
+#else
+#define PWM2_TMR __helper__(TC, PWM2_TIMER, )
+#define PWM2_CONFIG (                                \
+	{                                                \
+		PWM2_TMR-&gt;COUNT8.CTRLA.bit.SWRST = 1;        \
+		while (PWM2_TMR-&gt;COUNT8.STATUS.bit.SYNCBUSY) \
+			;                                        \
+		PWM2_TMR-&gt;COUNT8.CTRLA.bit.MODE = 1;         \
+		PWM2_TMR-&gt;COUNT8.CTRLA.bit.PRESCALER = 7;    \
+		PWM2_TMR-&gt;COUNT8.CTRLA.bit.WAVEGEN = 2;      \
+		while (PWM2_TMR-&gt;COUNT8.STATUS.bit.SYNCBUSY) \
+			;                                        \
+		PWM2_TMR-&gt;COUNT8.PER.reg = 255;              \
+		while (PWM2_TMR-&gt;COUNT8.STATUS.bit.SYNCBUSY) \
+			;                                        \
+		PWM2_TMR-&gt;COUNT8.CTRLA.bit.ENABLE = 1;       \
+		while (PWM2_TMR-&gt;COUNT8.STATUS.bit.SYNCBUSY) \
+			;                                        \
+	})
+#define PWM2_DUTYCYCLE (PWM2_TMR-&gt;COUNT8.CC[PWM2_CHANNEL].reg)
+#endif
+#define DIO22_PMUX PWM2_PMUX
+#define DIO22_PMUXVAL PWM2_PMUXVAL
+#define DIO22_TMR PWM2_TMR
+#define DIO22_CONFIG PWM2_CONFIG
+#define DIO22_DUTYCYCLE PWM2_DUTYCYCLE
+#endif</v>
+      </c>
+      <c r="I25" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>#if (defined(PWM2_OCR) &amp;&amp; defined(PWM2_TIMER) &amp;&amp; defined(PWM2))
-#define PWM2_OCRREG (__ocrreg__(PWM2_TIMER, PWM2_OCR))
-#define PWM2_TMRAREG (__tmrareg__(PWM2_TIMER))
-#define PWM2_TMRBREG (__tmrbreg__(PWM2_TIMER))
-#define PWM2_ENABLE_MASK __pwmenmask__(PWM2_OCR)
-#if (PWM2_TIMER == 2)
-#define PWM2_PRESCALLER 0x04
-#elif (PWM2_TIMER == 0)
-#define PWM2_PRESCALLER 0x03
-#else
-#define PWM2_PRESCALLER 0x0B
-#endif
-#if (PWM2_TIMER == 0 || PWM2_TIMER == 2)
-#define PWM2_MODE 0x03
-#else
-#define PWM2_MODE 0x01
-#endif
-#define DIO22_OCR PWM2_OCR
-#define DIO22_TIMER PWM2_TIMER
-#define DIO22_OCRREG PWM2_OCRREG
-#define DIO22_TMRAREG PWM2_TMRAREG
-#define DIO22_TMRBREG PWM2_TMRBREG
-#define DIO22_ENABLE_MASK PWM2_ENABLE_MASK
-#define DIO22_MODE PWM2_MODE
-#define DIO22_PRESCALLER PWM2_PRESCALLER
-#endif</v>
-      </c>
-      <c r="I25" s="3" t="str">
-        <f t="shared" si="5"/>
         <v>#ifdef PWM2
 mcu_config_pwm(PWM2);
 #endif</v>
@@ -39301,36 +39455,60 @@
       <c r="F26" s="6"/>
       <c r="G26" s="6"/>
       <c r="H26" s="6" t="str">
+        <f t="shared" si="5"/>
+        <v>#ifdef PWM3
+#define PWM3_CLKCTRL gclk_clkctrl(PWM3_TIMER)
+#define PWM3_PMUX (pinmux(PWM3_PORT, PWM3_BIT))
+#define PWM3_PMUXVAL (pinmuxval(PWM3_MUX))
+#if (PWM3_TIMER &lt; 3)
+#define PWM3_TMR __helper__(TCC, PWM3_TIMER, )
+#define PWM3_CONFIG (                         \
+	{                                         \
+		PWM3_TMR-&gt;CTRLA.bit.SWRST = 1;        \
+		while (PWM3_TMR-&gt;SYNCBUSY.bit.SWRST)  \
+			;                                 \
+		PWM3_TMR-&gt;CTRLA.bit.PRESCALER = 7;    \
+		PWM3_TMR-&gt;WAVE.bit.WAVEGEN = 2;       \
+		while (PWM3_TMR-&gt;SYNCBUSY.bit.WAVE)   \
+			;                                 \
+		PWM3_TMR-&gt;PER.bit.PER = 255;          \
+		while (PWM3_TMR-&gt;SYNCBUSY.bit.PER)    \
+			;                                 \
+		PWM3_TMR-&gt;CTRLA.bit.ENABLE = 1;       \
+		while (PWM3_TMR-&gt;SYNCBUSY.bit.ENABLE) \
+			;                                 \
+	})
+#define PWM3_DUTYCYCLE (PWM3_TMR-&gt;CC[PWM3_CHANNEL].bit.CC)
+#else
+#define PWM3_TMR __helper__(TC, PWM3_TIMER, )
+#define PWM3_CONFIG (                                \
+	{                                                \
+		PWM3_TMR-&gt;COUNT8.CTRLA.bit.SWRST = 1;        \
+		while (PWM3_TMR-&gt;COUNT8.STATUS.bit.SYNCBUSY) \
+			;                                        \
+		PWM3_TMR-&gt;COUNT8.CTRLA.bit.MODE = 1;         \
+		PWM3_TMR-&gt;COUNT8.CTRLA.bit.PRESCALER = 7;    \
+		PWM3_TMR-&gt;COUNT8.CTRLA.bit.WAVEGEN = 2;      \
+		while (PWM3_TMR-&gt;COUNT8.STATUS.bit.SYNCBUSY) \
+			;                                        \
+		PWM3_TMR-&gt;COUNT8.PER.reg = 255;              \
+		while (PWM3_TMR-&gt;COUNT8.STATUS.bit.SYNCBUSY) \
+			;                                        \
+		PWM3_TMR-&gt;COUNT8.CTRLA.bit.ENABLE = 1;       \
+		while (PWM3_TMR-&gt;COUNT8.STATUS.bit.SYNCBUSY) \
+			;                                        \
+	})
+#define PWM3_DUTYCYCLE (PWM3_TMR-&gt;COUNT8.CC[PWM3_CHANNEL].reg)
+#endif
+#define DIO23_PMUX PWM3_PMUX
+#define DIO23_PMUXVAL PWM3_PMUXVAL
+#define DIO23_TMR PWM3_TMR
+#define DIO23_CONFIG PWM3_CONFIG
+#define DIO23_DUTYCYCLE PWM3_DUTYCYCLE
+#endif</v>
+      </c>
+      <c r="I26" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>#if (defined(PWM3_OCR) &amp;&amp; defined(PWM3_TIMER) &amp;&amp; defined(PWM3))
-#define PWM3_OCRREG (__ocrreg__(PWM3_TIMER, PWM3_OCR))
-#define PWM3_TMRAREG (__tmrareg__(PWM3_TIMER))
-#define PWM3_TMRBREG (__tmrbreg__(PWM3_TIMER))
-#define PWM3_ENABLE_MASK __pwmenmask__(PWM3_OCR)
-#if (PWM3_TIMER == 2)
-#define PWM3_PRESCALLER 0x04
-#elif (PWM3_TIMER == 0)
-#define PWM3_PRESCALLER 0x03
-#else
-#define PWM3_PRESCALLER 0x0B
-#endif
-#if (PWM3_TIMER == 0 || PWM3_TIMER == 2)
-#define PWM3_MODE 0x03
-#else
-#define PWM3_MODE 0x01
-#endif
-#define DIO23_OCR PWM3_OCR
-#define DIO23_TIMER PWM3_TIMER
-#define DIO23_OCRREG PWM3_OCRREG
-#define DIO23_TMRAREG PWM3_TMRAREG
-#define DIO23_TMRBREG PWM3_TMRBREG
-#define DIO23_ENABLE_MASK PWM3_ENABLE_MASK
-#define DIO23_MODE PWM3_MODE
-#define DIO23_PRESCALLER PWM3_PRESCALLER
-#endif</v>
-      </c>
-      <c r="I26" s="3" t="str">
-        <f t="shared" si="5"/>
         <v>#ifdef PWM3
 mcu_config_pwm(PWM3);
 #endif</v>
@@ -39368,36 +39546,60 @@
       <c r="F27" s="6"/>
       <c r="G27" s="6"/>
       <c r="H27" s="6" t="str">
+        <f t="shared" si="5"/>
+        <v>#ifdef PWM4
+#define PWM4_CLKCTRL gclk_clkctrl(PWM4_TIMER)
+#define PWM4_PMUX (pinmux(PWM4_PORT, PWM4_BIT))
+#define PWM4_PMUXVAL (pinmuxval(PWM4_MUX))
+#if (PWM4_TIMER &lt; 3)
+#define PWM4_TMR __helper__(TCC, PWM4_TIMER, )
+#define PWM4_CONFIG (                         \
+	{                                         \
+		PWM4_TMR-&gt;CTRLA.bit.SWRST = 1;        \
+		while (PWM4_TMR-&gt;SYNCBUSY.bit.SWRST)  \
+			;                                 \
+		PWM4_TMR-&gt;CTRLA.bit.PRESCALER = 7;    \
+		PWM4_TMR-&gt;WAVE.bit.WAVEGEN = 2;       \
+		while (PWM4_TMR-&gt;SYNCBUSY.bit.WAVE)   \
+			;                                 \
+		PWM4_TMR-&gt;PER.bit.PER = 255;          \
+		while (PWM4_TMR-&gt;SYNCBUSY.bit.PER)    \
+			;                                 \
+		PWM4_TMR-&gt;CTRLA.bit.ENABLE = 1;       \
+		while (PWM4_TMR-&gt;SYNCBUSY.bit.ENABLE) \
+			;                                 \
+	})
+#define PWM4_DUTYCYCLE (PWM4_TMR-&gt;CC[PWM4_CHANNEL].bit.CC)
+#else
+#define PWM4_TMR __helper__(TC, PWM4_TIMER, )
+#define PWM4_CONFIG (                                \
+	{                                                \
+		PWM4_TMR-&gt;COUNT8.CTRLA.bit.SWRST = 1;        \
+		while (PWM4_TMR-&gt;COUNT8.STATUS.bit.SYNCBUSY) \
+			;                                        \
+		PWM4_TMR-&gt;COUNT8.CTRLA.bit.MODE = 1;         \
+		PWM4_TMR-&gt;COUNT8.CTRLA.bit.PRESCALER = 7;    \
+		PWM4_TMR-&gt;COUNT8.CTRLA.bit.WAVEGEN = 2;      \
+		while (PWM4_TMR-&gt;COUNT8.STATUS.bit.SYNCBUSY) \
+			;                                        \
+		PWM4_TMR-&gt;COUNT8.PER.reg = 255;              \
+		while (PWM4_TMR-&gt;COUNT8.STATUS.bit.SYNCBUSY) \
+			;                                        \
+		PWM4_TMR-&gt;COUNT8.CTRLA.bit.ENABLE = 1;       \
+		while (PWM4_TMR-&gt;COUNT8.STATUS.bit.SYNCBUSY) \
+			;                                        \
+	})
+#define PWM4_DUTYCYCLE (PWM4_TMR-&gt;COUNT8.CC[PWM4_CHANNEL].reg)
+#endif
+#define DIO24_PMUX PWM4_PMUX
+#define DIO24_PMUXVAL PWM4_PMUXVAL
+#define DIO24_TMR PWM4_TMR
+#define DIO24_CONFIG PWM4_CONFIG
+#define DIO24_DUTYCYCLE PWM4_DUTYCYCLE
+#endif</v>
+      </c>
+      <c r="I27" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>#if (defined(PWM4_OCR) &amp;&amp; defined(PWM4_TIMER) &amp;&amp; defined(PWM4))
-#define PWM4_OCRREG (__ocrreg__(PWM4_TIMER, PWM4_OCR))
-#define PWM4_TMRAREG (__tmrareg__(PWM4_TIMER))
-#define PWM4_TMRBREG (__tmrbreg__(PWM4_TIMER))
-#define PWM4_ENABLE_MASK __pwmenmask__(PWM4_OCR)
-#if (PWM4_TIMER == 2)
-#define PWM4_PRESCALLER 0x04
-#elif (PWM4_TIMER == 0)
-#define PWM4_PRESCALLER 0x03
-#else
-#define PWM4_PRESCALLER 0x0B
-#endif
-#if (PWM4_TIMER == 0 || PWM4_TIMER == 2)
-#define PWM4_MODE 0x03
-#else
-#define PWM4_MODE 0x01
-#endif
-#define DIO24_OCR PWM4_OCR
-#define DIO24_TIMER PWM4_TIMER
-#define DIO24_OCRREG PWM4_OCRREG
-#define DIO24_TMRAREG PWM4_TMRAREG
-#define DIO24_TMRBREG PWM4_TMRBREG
-#define DIO24_ENABLE_MASK PWM4_ENABLE_MASK
-#define DIO24_MODE PWM4_MODE
-#define DIO24_PRESCALLER PWM4_PRESCALLER
-#endif</v>
-      </c>
-      <c r="I27" s="3" t="str">
-        <f t="shared" si="5"/>
         <v>#ifdef PWM4
 mcu_config_pwm(PWM4);
 #endif</v>
@@ -39435,36 +39637,60 @@
       <c r="F28" s="6"/>
       <c r="G28" s="6"/>
       <c r="H28" s="6" t="str">
+        <f t="shared" si="5"/>
+        <v>#ifdef PWM5
+#define PWM5_CLKCTRL gclk_clkctrl(PWM5_TIMER)
+#define PWM5_PMUX (pinmux(PWM5_PORT, PWM5_BIT))
+#define PWM5_PMUXVAL (pinmuxval(PWM5_MUX))
+#if (PWM5_TIMER &lt; 3)
+#define PWM5_TMR __helper__(TCC, PWM5_TIMER, )
+#define PWM5_CONFIG (                         \
+	{                                         \
+		PWM5_TMR-&gt;CTRLA.bit.SWRST = 1;        \
+		while (PWM5_TMR-&gt;SYNCBUSY.bit.SWRST)  \
+			;                                 \
+		PWM5_TMR-&gt;CTRLA.bit.PRESCALER = 7;    \
+		PWM5_TMR-&gt;WAVE.bit.WAVEGEN = 2;       \
+		while (PWM5_TMR-&gt;SYNCBUSY.bit.WAVE)   \
+			;                                 \
+		PWM5_TMR-&gt;PER.bit.PER = 255;          \
+		while (PWM5_TMR-&gt;SYNCBUSY.bit.PER)    \
+			;                                 \
+		PWM5_TMR-&gt;CTRLA.bit.ENABLE = 1;       \
+		while (PWM5_TMR-&gt;SYNCBUSY.bit.ENABLE) \
+			;                                 \
+	})
+#define PWM5_DUTYCYCLE (PWM5_TMR-&gt;CC[PWM5_CHANNEL].bit.CC)
+#else
+#define PWM5_TMR __helper__(TC, PWM5_TIMER, )
+#define PWM5_CONFIG (                                \
+	{                                                \
+		PWM5_TMR-&gt;COUNT8.CTRLA.bit.SWRST = 1;        \
+		while (PWM5_TMR-&gt;COUNT8.STATUS.bit.SYNCBUSY) \
+			;                                        \
+		PWM5_TMR-&gt;COUNT8.CTRLA.bit.MODE = 1;         \
+		PWM5_TMR-&gt;COUNT8.CTRLA.bit.PRESCALER = 7;    \
+		PWM5_TMR-&gt;COUNT8.CTRLA.bit.WAVEGEN = 2;      \
+		while (PWM5_TMR-&gt;COUNT8.STATUS.bit.SYNCBUSY) \
+			;                                        \
+		PWM5_TMR-&gt;COUNT8.PER.reg = 255;              \
+		while (PWM5_TMR-&gt;COUNT8.STATUS.bit.SYNCBUSY) \
+			;                                        \
+		PWM5_TMR-&gt;COUNT8.CTRLA.bit.ENABLE = 1;       \
+		while (PWM5_TMR-&gt;COUNT8.STATUS.bit.SYNCBUSY) \
+			;                                        \
+	})
+#define PWM5_DUTYCYCLE (PWM5_TMR-&gt;COUNT8.CC[PWM5_CHANNEL].reg)
+#endif
+#define DIO25_PMUX PWM5_PMUX
+#define DIO25_PMUXVAL PWM5_PMUXVAL
+#define DIO25_TMR PWM5_TMR
+#define DIO25_CONFIG PWM5_CONFIG
+#define DIO25_DUTYCYCLE PWM5_DUTYCYCLE
+#endif</v>
+      </c>
+      <c r="I28" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>#if (defined(PWM5_OCR) &amp;&amp; defined(PWM5_TIMER) &amp;&amp; defined(PWM5))
-#define PWM5_OCRREG (__ocrreg__(PWM5_TIMER, PWM5_OCR))
-#define PWM5_TMRAREG (__tmrareg__(PWM5_TIMER))
-#define PWM5_TMRBREG (__tmrbreg__(PWM5_TIMER))
-#define PWM5_ENABLE_MASK __pwmenmask__(PWM5_OCR)
-#if (PWM5_TIMER == 2)
-#define PWM5_PRESCALLER 0x04
-#elif (PWM5_TIMER == 0)
-#define PWM5_PRESCALLER 0x03
-#else
-#define PWM5_PRESCALLER 0x0B
-#endif
-#if (PWM5_TIMER == 0 || PWM5_TIMER == 2)
-#define PWM5_MODE 0x03
-#else
-#define PWM5_MODE 0x01
-#endif
-#define DIO25_OCR PWM5_OCR
-#define DIO25_TIMER PWM5_TIMER
-#define DIO25_OCRREG PWM5_OCRREG
-#define DIO25_TMRAREG PWM5_TMRAREG
-#define DIO25_TMRBREG PWM5_TMRBREG
-#define DIO25_ENABLE_MASK PWM5_ENABLE_MASK
-#define DIO25_MODE PWM5_MODE
-#define DIO25_PRESCALLER PWM5_PRESCALLER
-#endif</v>
-      </c>
-      <c r="I28" s="3" t="str">
-        <f t="shared" si="5"/>
         <v>#ifdef PWM5
 mcu_config_pwm(PWM5);
 #endif</v>
@@ -39502,36 +39728,60 @@
       <c r="F29" s="6"/>
       <c r="G29" s="6"/>
       <c r="H29" s="6" t="str">
+        <f t="shared" si="5"/>
+        <v>#ifdef PWM6
+#define PWM6_CLKCTRL gclk_clkctrl(PWM6_TIMER)
+#define PWM6_PMUX (pinmux(PWM6_PORT, PWM6_BIT))
+#define PWM6_PMUXVAL (pinmuxval(PWM6_MUX))
+#if (PWM6_TIMER &lt; 3)
+#define PWM6_TMR __helper__(TCC, PWM6_TIMER, )
+#define PWM6_CONFIG (                         \
+	{                                         \
+		PWM6_TMR-&gt;CTRLA.bit.SWRST = 1;        \
+		while (PWM6_TMR-&gt;SYNCBUSY.bit.SWRST)  \
+			;                                 \
+		PWM6_TMR-&gt;CTRLA.bit.PRESCALER = 7;    \
+		PWM6_TMR-&gt;WAVE.bit.WAVEGEN = 2;       \
+		while (PWM6_TMR-&gt;SYNCBUSY.bit.WAVE)   \
+			;                                 \
+		PWM6_TMR-&gt;PER.bit.PER = 255;          \
+		while (PWM6_TMR-&gt;SYNCBUSY.bit.PER)    \
+			;                                 \
+		PWM6_TMR-&gt;CTRLA.bit.ENABLE = 1;       \
+		while (PWM6_TMR-&gt;SYNCBUSY.bit.ENABLE) \
+			;                                 \
+	})
+#define PWM6_DUTYCYCLE (PWM6_TMR-&gt;CC[PWM6_CHANNEL].bit.CC)
+#else
+#define PWM6_TMR __helper__(TC, PWM6_TIMER, )
+#define PWM6_CONFIG (                                \
+	{                                                \
+		PWM6_TMR-&gt;COUNT8.CTRLA.bit.SWRST = 1;        \
+		while (PWM6_TMR-&gt;COUNT8.STATUS.bit.SYNCBUSY) \
+			;                                        \
+		PWM6_TMR-&gt;COUNT8.CTRLA.bit.MODE = 1;         \
+		PWM6_TMR-&gt;COUNT8.CTRLA.bit.PRESCALER = 7;    \
+		PWM6_TMR-&gt;COUNT8.CTRLA.bit.WAVEGEN = 2;      \
+		while (PWM6_TMR-&gt;COUNT8.STATUS.bit.SYNCBUSY) \
+			;                                        \
+		PWM6_TMR-&gt;COUNT8.PER.reg = 255;              \
+		while (PWM6_TMR-&gt;COUNT8.STATUS.bit.SYNCBUSY) \
+			;                                        \
+		PWM6_TMR-&gt;COUNT8.CTRLA.bit.ENABLE = 1;       \
+		while (PWM6_TMR-&gt;COUNT8.STATUS.bit.SYNCBUSY) \
+			;                                        \
+	})
+#define PWM6_DUTYCYCLE (PWM6_TMR-&gt;COUNT8.CC[PWM6_CHANNEL].reg)
+#endif
+#define DIO26_PMUX PWM6_PMUX
+#define DIO26_PMUXVAL PWM6_PMUXVAL
+#define DIO26_TMR PWM6_TMR
+#define DIO26_CONFIG PWM6_CONFIG
+#define DIO26_DUTYCYCLE PWM6_DUTYCYCLE
+#endif</v>
+      </c>
+      <c r="I29" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>#if (defined(PWM6_OCR) &amp;&amp; defined(PWM6_TIMER) &amp;&amp; defined(PWM6))
-#define PWM6_OCRREG (__ocrreg__(PWM6_TIMER, PWM6_OCR))
-#define PWM6_TMRAREG (__tmrareg__(PWM6_TIMER))
-#define PWM6_TMRBREG (__tmrbreg__(PWM6_TIMER))
-#define PWM6_ENABLE_MASK __pwmenmask__(PWM6_OCR)
-#if (PWM6_TIMER == 2)
-#define PWM6_PRESCALLER 0x04
-#elif (PWM6_TIMER == 0)
-#define PWM6_PRESCALLER 0x03
-#else
-#define PWM6_PRESCALLER 0x0B
-#endif
-#if (PWM6_TIMER == 0 || PWM6_TIMER == 2)
-#define PWM6_MODE 0x03
-#else
-#define PWM6_MODE 0x01
-#endif
-#define DIO26_OCR PWM6_OCR
-#define DIO26_TIMER PWM6_TIMER
-#define DIO26_OCRREG PWM6_OCRREG
-#define DIO26_TMRAREG PWM6_TMRAREG
-#define DIO26_TMRBREG PWM6_TMRBREG
-#define DIO26_ENABLE_MASK PWM6_ENABLE_MASK
-#define DIO26_MODE PWM6_MODE
-#define DIO26_PRESCALLER PWM6_PRESCALLER
-#endif</v>
-      </c>
-      <c r="I29" s="3" t="str">
-        <f t="shared" si="5"/>
         <v>#ifdef PWM6
 mcu_config_pwm(PWM6);
 #endif</v>
@@ -39569,36 +39819,60 @@
       <c r="F30" s="6"/>
       <c r="G30" s="6"/>
       <c r="H30" s="6" t="str">
+        <f t="shared" si="5"/>
+        <v>#ifdef PWM7
+#define PWM7_CLKCTRL gclk_clkctrl(PWM7_TIMER)
+#define PWM7_PMUX (pinmux(PWM7_PORT, PWM7_BIT))
+#define PWM7_PMUXVAL (pinmuxval(PWM7_MUX))
+#if (PWM7_TIMER &lt; 3)
+#define PWM7_TMR __helper__(TCC, PWM7_TIMER, )
+#define PWM7_CONFIG (                         \
+	{                                         \
+		PWM7_TMR-&gt;CTRLA.bit.SWRST = 1;        \
+		while (PWM7_TMR-&gt;SYNCBUSY.bit.SWRST)  \
+			;                                 \
+		PWM7_TMR-&gt;CTRLA.bit.PRESCALER = 7;    \
+		PWM7_TMR-&gt;WAVE.bit.WAVEGEN = 2;       \
+		while (PWM7_TMR-&gt;SYNCBUSY.bit.WAVE)   \
+			;                                 \
+		PWM7_TMR-&gt;PER.bit.PER = 255;          \
+		while (PWM7_TMR-&gt;SYNCBUSY.bit.PER)    \
+			;                                 \
+		PWM7_TMR-&gt;CTRLA.bit.ENABLE = 1;       \
+		while (PWM7_TMR-&gt;SYNCBUSY.bit.ENABLE) \
+			;                                 \
+	})
+#define PWM7_DUTYCYCLE (PWM7_TMR-&gt;CC[PWM7_CHANNEL].bit.CC)
+#else
+#define PWM7_TMR __helper__(TC, PWM7_TIMER, )
+#define PWM7_CONFIG (                                \
+	{                                                \
+		PWM7_TMR-&gt;COUNT8.CTRLA.bit.SWRST = 1;        \
+		while (PWM7_TMR-&gt;COUNT8.STATUS.bit.SYNCBUSY) \
+			;                                        \
+		PWM7_TMR-&gt;COUNT8.CTRLA.bit.MODE = 1;         \
+		PWM7_TMR-&gt;COUNT8.CTRLA.bit.PRESCALER = 7;    \
+		PWM7_TMR-&gt;COUNT8.CTRLA.bit.WAVEGEN = 2;      \
+		while (PWM7_TMR-&gt;COUNT8.STATUS.bit.SYNCBUSY) \
+			;                                        \
+		PWM7_TMR-&gt;COUNT8.PER.reg = 255;              \
+		while (PWM7_TMR-&gt;COUNT8.STATUS.bit.SYNCBUSY) \
+			;                                        \
+		PWM7_TMR-&gt;COUNT8.CTRLA.bit.ENABLE = 1;       \
+		while (PWM7_TMR-&gt;COUNT8.STATUS.bit.SYNCBUSY) \
+			;                                        \
+	})
+#define PWM7_DUTYCYCLE (PWM7_TMR-&gt;COUNT8.CC[PWM7_CHANNEL].reg)
+#endif
+#define DIO27_PMUX PWM7_PMUX
+#define DIO27_PMUXVAL PWM7_PMUXVAL
+#define DIO27_TMR PWM7_TMR
+#define DIO27_CONFIG PWM7_CONFIG
+#define DIO27_DUTYCYCLE PWM7_DUTYCYCLE
+#endif</v>
+      </c>
+      <c r="I30" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>#if (defined(PWM7_OCR) &amp;&amp; defined(PWM7_TIMER) &amp;&amp; defined(PWM7))
-#define PWM7_OCRREG (__ocrreg__(PWM7_TIMER, PWM7_OCR))
-#define PWM7_TMRAREG (__tmrareg__(PWM7_TIMER))
-#define PWM7_TMRBREG (__tmrbreg__(PWM7_TIMER))
-#define PWM7_ENABLE_MASK __pwmenmask__(PWM7_OCR)
-#if (PWM7_TIMER == 2)
-#define PWM7_PRESCALLER 0x04
-#elif (PWM7_TIMER == 0)
-#define PWM7_PRESCALLER 0x03
-#else
-#define PWM7_PRESCALLER 0x0B
-#endif
-#if (PWM7_TIMER == 0 || PWM7_TIMER == 2)
-#define PWM7_MODE 0x03
-#else
-#define PWM7_MODE 0x01
-#endif
-#define DIO27_OCR PWM7_OCR
-#define DIO27_TIMER PWM7_TIMER
-#define DIO27_OCRREG PWM7_OCRREG
-#define DIO27_TMRAREG PWM7_TMRAREG
-#define DIO27_TMRBREG PWM7_TMRBREG
-#define DIO27_ENABLE_MASK PWM7_ENABLE_MASK
-#define DIO27_MODE PWM7_MODE
-#define DIO27_PRESCALLER PWM7_PRESCALLER
-#endif</v>
-      </c>
-      <c r="I30" s="3" t="str">
-        <f t="shared" si="5"/>
         <v>#ifdef PWM7
 mcu_config_pwm(PWM7);
 #endif</v>
@@ -39636,36 +39910,60 @@
       <c r="F31" s="6"/>
       <c r="G31" s="6"/>
       <c r="H31" s="6" t="str">
+        <f t="shared" si="5"/>
+        <v>#ifdef PWM8
+#define PWM8_CLKCTRL gclk_clkctrl(PWM8_TIMER)
+#define PWM8_PMUX (pinmux(PWM8_PORT, PWM8_BIT))
+#define PWM8_PMUXVAL (pinmuxval(PWM8_MUX))
+#if (PWM8_TIMER &lt; 3)
+#define PWM8_TMR __helper__(TCC, PWM8_TIMER, )
+#define PWM8_CONFIG (                         \
+	{                                         \
+		PWM8_TMR-&gt;CTRLA.bit.SWRST = 1;        \
+		while (PWM8_TMR-&gt;SYNCBUSY.bit.SWRST)  \
+			;                                 \
+		PWM8_TMR-&gt;CTRLA.bit.PRESCALER = 7;    \
+		PWM8_TMR-&gt;WAVE.bit.WAVEGEN = 2;       \
+		while (PWM8_TMR-&gt;SYNCBUSY.bit.WAVE)   \
+			;                                 \
+		PWM8_TMR-&gt;PER.bit.PER = 255;          \
+		while (PWM8_TMR-&gt;SYNCBUSY.bit.PER)    \
+			;                                 \
+		PWM8_TMR-&gt;CTRLA.bit.ENABLE = 1;       \
+		while (PWM8_TMR-&gt;SYNCBUSY.bit.ENABLE) \
+			;                                 \
+	})
+#define PWM8_DUTYCYCLE (PWM8_TMR-&gt;CC[PWM8_CHANNEL].bit.CC)
+#else
+#define PWM8_TMR __helper__(TC, PWM8_TIMER, )
+#define PWM8_CONFIG (                                \
+	{                                                \
+		PWM8_TMR-&gt;COUNT8.CTRLA.bit.SWRST = 1;        \
+		while (PWM8_TMR-&gt;COUNT8.STATUS.bit.SYNCBUSY) \
+			;                                        \
+		PWM8_TMR-&gt;COUNT8.CTRLA.bit.MODE = 1;         \
+		PWM8_TMR-&gt;COUNT8.CTRLA.bit.PRESCALER = 7;    \
+		PWM8_TMR-&gt;COUNT8.CTRLA.bit.WAVEGEN = 2;      \
+		while (PWM8_TMR-&gt;COUNT8.STATUS.bit.SYNCBUSY) \
+			;                                        \
+		PWM8_TMR-&gt;COUNT8.PER.reg = 255;              \
+		while (PWM8_TMR-&gt;COUNT8.STATUS.bit.SYNCBUSY) \
+			;                                        \
+		PWM8_TMR-&gt;COUNT8.CTRLA.bit.ENABLE = 1;       \
+		while (PWM8_TMR-&gt;COUNT8.STATUS.bit.SYNCBUSY) \
+			;                                        \
+	})
+#define PWM8_DUTYCYCLE (PWM8_TMR-&gt;COUNT8.CC[PWM8_CHANNEL].reg)
+#endif
+#define DIO28_PMUX PWM8_PMUX
+#define DIO28_PMUXVAL PWM8_PMUXVAL
+#define DIO28_TMR PWM8_TMR
+#define DIO28_CONFIG PWM8_CONFIG
+#define DIO28_DUTYCYCLE PWM8_DUTYCYCLE
+#endif</v>
+      </c>
+      <c r="I31" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>#if (defined(PWM8_OCR) &amp;&amp; defined(PWM8_TIMER) &amp;&amp; defined(PWM8))
-#define PWM8_OCRREG (__ocrreg__(PWM8_TIMER, PWM8_OCR))
-#define PWM8_TMRAREG (__tmrareg__(PWM8_TIMER))
-#define PWM8_TMRBREG (__tmrbreg__(PWM8_TIMER))
-#define PWM8_ENABLE_MASK __pwmenmask__(PWM8_OCR)
-#if (PWM8_TIMER == 2)
-#define PWM8_PRESCALLER 0x04
-#elif (PWM8_TIMER == 0)
-#define PWM8_PRESCALLER 0x03
-#else
-#define PWM8_PRESCALLER 0x0B
-#endif
-#if (PWM8_TIMER == 0 || PWM8_TIMER == 2)
-#define PWM8_MODE 0x03
-#else
-#define PWM8_MODE 0x01
-#endif
-#define DIO28_OCR PWM8_OCR
-#define DIO28_TIMER PWM8_TIMER
-#define DIO28_OCRREG PWM8_OCRREG
-#define DIO28_TMRAREG PWM8_TMRAREG
-#define DIO28_TMRBREG PWM8_TMRBREG
-#define DIO28_ENABLE_MASK PWM8_ENABLE_MASK
-#define DIO28_MODE PWM8_MODE
-#define DIO28_PRESCALLER PWM8_PRESCALLER
-#endif</v>
-      </c>
-      <c r="I31" s="3" t="str">
-        <f t="shared" si="5"/>
         <v>#ifdef PWM8
 mcu_config_pwm(PWM8);
 #endif</v>
@@ -39703,36 +40001,60 @@
       <c r="F32" s="6"/>
       <c r="G32" s="6"/>
       <c r="H32" s="6" t="str">
+        <f t="shared" si="5"/>
+        <v>#ifdef PWM9
+#define PWM9_CLKCTRL gclk_clkctrl(PWM9_TIMER)
+#define PWM9_PMUX (pinmux(PWM9_PORT, PWM9_BIT))
+#define PWM9_PMUXVAL (pinmuxval(PWM9_MUX))
+#if (PWM9_TIMER &lt; 3)
+#define PWM9_TMR __helper__(TCC, PWM9_TIMER, )
+#define PWM9_CONFIG (                         \
+	{                                         \
+		PWM9_TMR-&gt;CTRLA.bit.SWRST = 1;        \
+		while (PWM9_TMR-&gt;SYNCBUSY.bit.SWRST)  \
+			;                                 \
+		PWM9_TMR-&gt;CTRLA.bit.PRESCALER = 7;    \
+		PWM9_TMR-&gt;WAVE.bit.WAVEGEN = 2;       \
+		while (PWM9_TMR-&gt;SYNCBUSY.bit.WAVE)   \
+			;                                 \
+		PWM9_TMR-&gt;PER.bit.PER = 255;          \
+		while (PWM9_TMR-&gt;SYNCBUSY.bit.PER)    \
+			;                                 \
+		PWM9_TMR-&gt;CTRLA.bit.ENABLE = 1;       \
+		while (PWM9_TMR-&gt;SYNCBUSY.bit.ENABLE) \
+			;                                 \
+	})
+#define PWM9_DUTYCYCLE (PWM9_TMR-&gt;CC[PWM9_CHANNEL].bit.CC)
+#else
+#define PWM9_TMR __helper__(TC, PWM9_TIMER, )
+#define PWM9_CONFIG (                                \
+	{                                                \
+		PWM9_TMR-&gt;COUNT8.CTRLA.bit.SWRST = 1;        \
+		while (PWM9_TMR-&gt;COUNT8.STATUS.bit.SYNCBUSY) \
+			;                                        \
+		PWM9_TMR-&gt;COUNT8.CTRLA.bit.MODE = 1;         \
+		PWM9_TMR-&gt;COUNT8.CTRLA.bit.PRESCALER = 7;    \
+		PWM9_TMR-&gt;COUNT8.CTRLA.bit.WAVEGEN = 2;      \
+		while (PWM9_TMR-&gt;COUNT8.STATUS.bit.SYNCBUSY) \
+			;                                        \
+		PWM9_TMR-&gt;COUNT8.PER.reg = 255;              \
+		while (PWM9_TMR-&gt;COUNT8.STATUS.bit.SYNCBUSY) \
+			;                                        \
+		PWM9_TMR-&gt;COUNT8.CTRLA.bit.ENABLE = 1;       \
+		while (PWM9_TMR-&gt;COUNT8.STATUS.bit.SYNCBUSY) \
+			;                                        \
+	})
+#define PWM9_DUTYCYCLE (PWM9_TMR-&gt;COUNT8.CC[PWM9_CHANNEL].reg)
+#endif
+#define DIO29_PMUX PWM9_PMUX
+#define DIO29_PMUXVAL PWM9_PMUXVAL
+#define DIO29_TMR PWM9_TMR
+#define DIO29_CONFIG PWM9_CONFIG
+#define DIO29_DUTYCYCLE PWM9_DUTYCYCLE
+#endif</v>
+      </c>
+      <c r="I32" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>#if (defined(PWM9_OCR) &amp;&amp; defined(PWM9_TIMER) &amp;&amp; defined(PWM9))
-#define PWM9_OCRREG (__ocrreg__(PWM9_TIMER, PWM9_OCR))
-#define PWM9_TMRAREG (__tmrareg__(PWM9_TIMER))
-#define PWM9_TMRBREG (__tmrbreg__(PWM9_TIMER))
-#define PWM9_ENABLE_MASK __pwmenmask__(PWM9_OCR)
-#if (PWM9_TIMER == 2)
-#define PWM9_PRESCALLER 0x04
-#elif (PWM9_TIMER == 0)
-#define PWM9_PRESCALLER 0x03
-#else
-#define PWM9_PRESCALLER 0x0B
-#endif
-#if (PWM9_TIMER == 0 || PWM9_TIMER == 2)
-#define PWM9_MODE 0x03
-#else
-#define PWM9_MODE 0x01
-#endif
-#define DIO29_OCR PWM9_OCR
-#define DIO29_TIMER PWM9_TIMER
-#define DIO29_OCRREG PWM9_OCRREG
-#define DIO29_TMRAREG PWM9_TMRAREG
-#define DIO29_TMRBREG PWM9_TMRBREG
-#define DIO29_ENABLE_MASK PWM9_ENABLE_MASK
-#define DIO29_MODE PWM9_MODE
-#define DIO29_PRESCALLER PWM9_PRESCALLER
-#endif</v>
-      </c>
-      <c r="I32" s="3" t="str">
-        <f t="shared" si="5"/>
         <v>#ifdef PWM9
 mcu_config_pwm(PWM9);
 #endif</v>
@@ -39770,36 +40092,60 @@
       <c r="F33" s="6"/>
       <c r="G33" s="6"/>
       <c r="H33" s="6" t="str">
+        <f t="shared" si="5"/>
+        <v>#ifdef PWM10
+#define PWM10_CLKCTRL gclk_clkctrl(PWM10_TIMER)
+#define PWM10_PMUX (pinmux(PWM10_PORT, PWM10_BIT))
+#define PWM10_PMUXVAL (pinmuxval(PWM10_MUX))
+#if (PWM10_TIMER &lt; 3)
+#define PWM10_TMR __helper__(TCC, PWM10_TIMER, )
+#define PWM10_CONFIG (                         \
+	{                                         \
+		PWM10_TMR-&gt;CTRLA.bit.SWRST = 1;        \
+		while (PWM10_TMR-&gt;SYNCBUSY.bit.SWRST)  \
+			;                                 \
+		PWM10_TMR-&gt;CTRLA.bit.PRESCALER = 7;    \
+		PWM10_TMR-&gt;WAVE.bit.WAVEGEN = 2;       \
+		while (PWM10_TMR-&gt;SYNCBUSY.bit.WAVE)   \
+			;                                 \
+		PWM10_TMR-&gt;PER.bit.PER = 255;          \
+		while (PWM10_TMR-&gt;SYNCBUSY.bit.PER)    \
+			;                                 \
+		PWM10_TMR-&gt;CTRLA.bit.ENABLE = 1;       \
+		while (PWM10_TMR-&gt;SYNCBUSY.bit.ENABLE) \
+			;                                 \
+	})
+#define PWM10_DUTYCYCLE (PWM10_TMR-&gt;CC[PWM10_CHANNEL].bit.CC)
+#else
+#define PWM10_TMR __helper__(TC, PWM10_TIMER, )
+#define PWM10_CONFIG (                                \
+	{                                                \
+		PWM10_TMR-&gt;COUNT8.CTRLA.bit.SWRST = 1;        \
+		while (PWM10_TMR-&gt;COUNT8.STATUS.bit.SYNCBUSY) \
+			;                                        \
+		PWM10_TMR-&gt;COUNT8.CTRLA.bit.MODE = 1;         \
+		PWM10_TMR-&gt;COUNT8.CTRLA.bit.PRESCALER = 7;    \
+		PWM10_TMR-&gt;COUNT8.CTRLA.bit.WAVEGEN = 2;      \
+		while (PWM10_TMR-&gt;COUNT8.STATUS.bit.SYNCBUSY) \
+			;                                        \
+		PWM10_TMR-&gt;COUNT8.PER.reg = 255;              \
+		while (PWM10_TMR-&gt;COUNT8.STATUS.bit.SYNCBUSY) \
+			;                                        \
+		PWM10_TMR-&gt;COUNT8.CTRLA.bit.ENABLE = 1;       \
+		while (PWM10_TMR-&gt;COUNT8.STATUS.bit.SYNCBUSY) \
+			;                                        \
+	})
+#define PWM10_DUTYCYCLE (PWM10_TMR-&gt;COUNT8.CC[PWM10_CHANNEL].reg)
+#endif
+#define DIO30_PMUX PWM10_PMUX
+#define DIO30_PMUXVAL PWM10_PMUXVAL
+#define DIO30_TMR PWM10_TMR
+#define DIO30_CONFIG PWM10_CONFIG
+#define DIO30_DUTYCYCLE PWM10_DUTYCYCLE
+#endif</v>
+      </c>
+      <c r="I33" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>#if (defined(PWM10_OCR) &amp;&amp; defined(PWM10_TIMER) &amp;&amp; defined(PWM10))
-#define PWM10_OCRREG (__ocrreg__(PWM10_TIMER, PWM10_OCR))
-#define PWM10_TMRAREG (__tmrareg__(PWM10_TIMER))
-#define PWM10_TMRBREG (__tmrbreg__(PWM10_TIMER))
-#define PWM10_ENABLE_MASK __pwmenmask__(PWM10_OCR)
-#if (PWM10_TIMER == 2)
-#define PWM10_PRESCALLER 0x04
-#elif (PWM10_TIMER == 0)
-#define PWM10_PRESCALLER 0x03
-#else
-#define PWM10_PRESCALLER 0x0B
-#endif
-#if (PWM10_TIMER == 0 || PWM10_TIMER == 2)
-#define PWM10_MODE 0x03
-#else
-#define PWM10_MODE 0x01
-#endif
-#define DIO30_OCR PWM10_OCR
-#define DIO30_TIMER PWM10_TIMER
-#define DIO30_OCRREG PWM10_OCRREG
-#define DIO30_TMRAREG PWM10_TMRAREG
-#define DIO30_TMRBREG PWM10_TMRBREG
-#define DIO30_ENABLE_MASK PWM10_ENABLE_MASK
-#define DIO30_MODE PWM10_MODE
-#define DIO30_PRESCALLER PWM10_PRESCALLER
-#endif</v>
-      </c>
-      <c r="I33" s="3" t="str">
-        <f t="shared" si="5"/>
         <v>#ifdef PWM10
 mcu_config_pwm(PWM10);
 #endif</v>
@@ -39837,36 +40183,60 @@
       <c r="F34" s="6"/>
       <c r="G34" s="6"/>
       <c r="H34" s="6" t="str">
+        <f t="shared" si="5"/>
+        <v>#ifdef PWM11
+#define PWM11_CLKCTRL gclk_clkctrl(PWM11_TIMER)
+#define PWM11_PMUX (pinmux(PWM11_PORT, PWM11_BIT))
+#define PWM11_PMUXVAL (pinmuxval(PWM11_MUX))
+#if (PWM11_TIMER &lt; 3)
+#define PWM11_TMR __helper__(TCC, PWM11_TIMER, )
+#define PWM11_CONFIG (                         \
+	{                                         \
+		PWM11_TMR-&gt;CTRLA.bit.SWRST = 1;        \
+		while (PWM11_TMR-&gt;SYNCBUSY.bit.SWRST)  \
+			;                                 \
+		PWM11_TMR-&gt;CTRLA.bit.PRESCALER = 7;    \
+		PWM11_TMR-&gt;WAVE.bit.WAVEGEN = 2;       \
+		while (PWM11_TMR-&gt;SYNCBUSY.bit.WAVE)   \
+			;                                 \
+		PWM11_TMR-&gt;PER.bit.PER = 255;          \
+		while (PWM11_TMR-&gt;SYNCBUSY.bit.PER)    \
+			;                                 \
+		PWM11_TMR-&gt;CTRLA.bit.ENABLE = 1;       \
+		while (PWM11_TMR-&gt;SYNCBUSY.bit.ENABLE) \
+			;                                 \
+	})
+#define PWM11_DUTYCYCLE (PWM11_TMR-&gt;CC[PWM11_CHANNEL].bit.CC)
+#else
+#define PWM11_TMR __helper__(TC, PWM11_TIMER, )
+#define PWM11_CONFIG (                                \
+	{                                                \
+		PWM11_TMR-&gt;COUNT8.CTRLA.bit.SWRST = 1;        \
+		while (PWM11_TMR-&gt;COUNT8.STATUS.bit.SYNCBUSY) \
+			;                                        \
+		PWM11_TMR-&gt;COUNT8.CTRLA.bit.MODE = 1;         \
+		PWM11_TMR-&gt;COUNT8.CTRLA.bit.PRESCALER = 7;    \
+		PWM11_TMR-&gt;COUNT8.CTRLA.bit.WAVEGEN = 2;      \
+		while (PWM11_TMR-&gt;COUNT8.STATUS.bit.SYNCBUSY) \
+			;                                        \
+		PWM11_TMR-&gt;COUNT8.PER.reg = 255;              \
+		while (PWM11_TMR-&gt;COUNT8.STATUS.bit.SYNCBUSY) \
+			;                                        \
+		PWM11_TMR-&gt;COUNT8.CTRLA.bit.ENABLE = 1;       \
+		while (PWM11_TMR-&gt;COUNT8.STATUS.bit.SYNCBUSY) \
+			;                                        \
+	})
+#define PWM11_DUTYCYCLE (PWM11_TMR-&gt;COUNT8.CC[PWM11_CHANNEL].reg)
+#endif
+#define DIO31_PMUX PWM11_PMUX
+#define DIO31_PMUXVAL PWM11_PMUXVAL
+#define DIO31_TMR PWM11_TMR
+#define DIO31_CONFIG PWM11_CONFIG
+#define DIO31_DUTYCYCLE PWM11_DUTYCYCLE
+#endif</v>
+      </c>
+      <c r="I34" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>#if (defined(PWM11_OCR) &amp;&amp; defined(PWM11_TIMER) &amp;&amp; defined(PWM11))
-#define PWM11_OCRREG (__ocrreg__(PWM11_TIMER, PWM11_OCR))
-#define PWM11_TMRAREG (__tmrareg__(PWM11_TIMER))
-#define PWM11_TMRBREG (__tmrbreg__(PWM11_TIMER))
-#define PWM11_ENABLE_MASK __pwmenmask__(PWM11_OCR)
-#if (PWM11_TIMER == 2)
-#define PWM11_PRESCALLER 0x04
-#elif (PWM11_TIMER == 0)
-#define PWM11_PRESCALLER 0x03
-#else
-#define PWM11_PRESCALLER 0x0B
-#endif
-#if (PWM11_TIMER == 0 || PWM11_TIMER == 2)
-#define PWM11_MODE 0x03
-#else
-#define PWM11_MODE 0x01
-#endif
-#define DIO31_OCR PWM11_OCR
-#define DIO31_TIMER PWM11_TIMER
-#define DIO31_OCRREG PWM11_OCRREG
-#define DIO31_TMRAREG PWM11_TMRAREG
-#define DIO31_TMRBREG PWM11_TMRBREG
-#define DIO31_ENABLE_MASK PWM11_ENABLE_MASK
-#define DIO31_MODE PWM11_MODE
-#define DIO31_PRESCALLER PWM11_PRESCALLER
-#endif</v>
-      </c>
-      <c r="I34" s="3" t="str">
-        <f t="shared" si="5"/>
         <v>#ifdef PWM11
 mcu_config_pwm(PWM11);
 #endif</v>
@@ -39904,36 +40274,60 @@
       <c r="F35" s="6"/>
       <c r="G35" s="6"/>
       <c r="H35" s="6" t="str">
+        <f t="shared" si="5"/>
+        <v>#ifdef PWM12
+#define PWM12_CLKCTRL gclk_clkctrl(PWM12_TIMER)
+#define PWM12_PMUX (pinmux(PWM12_PORT, PWM12_BIT))
+#define PWM12_PMUXVAL (pinmuxval(PWM12_MUX))
+#if (PWM12_TIMER &lt; 3)
+#define PWM12_TMR __helper__(TCC, PWM12_TIMER, )
+#define PWM12_CONFIG (                         \
+	{                                         \
+		PWM12_TMR-&gt;CTRLA.bit.SWRST = 1;        \
+		while (PWM12_TMR-&gt;SYNCBUSY.bit.SWRST)  \
+			;                                 \
+		PWM12_TMR-&gt;CTRLA.bit.PRESCALER = 7;    \
+		PWM12_TMR-&gt;WAVE.bit.WAVEGEN = 2;       \
+		while (PWM12_TMR-&gt;SYNCBUSY.bit.WAVE)   \
+			;                                 \
+		PWM12_TMR-&gt;PER.bit.PER = 255;          \
+		while (PWM12_TMR-&gt;SYNCBUSY.bit.PER)    \
+			;                                 \
+		PWM12_TMR-&gt;CTRLA.bit.ENABLE = 1;       \
+		while (PWM12_TMR-&gt;SYNCBUSY.bit.ENABLE) \
+			;                                 \
+	})
+#define PWM12_DUTYCYCLE (PWM12_TMR-&gt;CC[PWM12_CHANNEL].bit.CC)
+#else
+#define PWM12_TMR __helper__(TC, PWM12_TIMER, )
+#define PWM12_CONFIG (                                \
+	{                                                \
+		PWM12_TMR-&gt;COUNT8.CTRLA.bit.SWRST = 1;        \
+		while (PWM12_TMR-&gt;COUNT8.STATUS.bit.SYNCBUSY) \
+			;                                        \
+		PWM12_TMR-&gt;COUNT8.CTRLA.bit.MODE = 1;         \
+		PWM12_TMR-&gt;COUNT8.CTRLA.bit.PRESCALER = 7;    \
+		PWM12_TMR-&gt;COUNT8.CTRLA.bit.WAVEGEN = 2;      \
+		while (PWM12_TMR-&gt;COUNT8.STATUS.bit.SYNCBUSY) \
+			;                                        \
+		PWM12_TMR-&gt;COUNT8.PER.reg = 255;              \
+		while (PWM12_TMR-&gt;COUNT8.STATUS.bit.SYNCBUSY) \
+			;                                        \
+		PWM12_TMR-&gt;COUNT8.CTRLA.bit.ENABLE = 1;       \
+		while (PWM12_TMR-&gt;COUNT8.STATUS.bit.SYNCBUSY) \
+			;                                        \
+	})
+#define PWM12_DUTYCYCLE (PWM12_TMR-&gt;COUNT8.CC[PWM12_CHANNEL].reg)
+#endif
+#define DIO32_PMUX PWM12_PMUX
+#define DIO32_PMUXVAL PWM12_PMUXVAL
+#define DIO32_TMR PWM12_TMR
+#define DIO32_CONFIG PWM12_CONFIG
+#define DIO32_DUTYCYCLE PWM12_DUTYCYCLE
+#endif</v>
+      </c>
+      <c r="I35" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>#if (defined(PWM12_OCR) &amp;&amp; defined(PWM12_TIMER) &amp;&amp; defined(PWM12))
-#define PWM12_OCRREG (__ocrreg__(PWM12_TIMER, PWM12_OCR))
-#define PWM12_TMRAREG (__tmrareg__(PWM12_TIMER))
-#define PWM12_TMRBREG (__tmrbreg__(PWM12_TIMER))
-#define PWM12_ENABLE_MASK __pwmenmask__(PWM12_OCR)
-#if (PWM12_TIMER == 2)
-#define PWM12_PRESCALLER 0x04
-#elif (PWM12_TIMER == 0)
-#define PWM12_PRESCALLER 0x03
-#else
-#define PWM12_PRESCALLER 0x0B
-#endif
-#if (PWM12_TIMER == 0 || PWM12_TIMER == 2)
-#define PWM12_MODE 0x03
-#else
-#define PWM12_MODE 0x01
-#endif
-#define DIO32_OCR PWM12_OCR
-#define DIO32_TIMER PWM12_TIMER
-#define DIO32_OCRREG PWM12_OCRREG
-#define DIO32_TMRAREG PWM12_TMRAREG
-#define DIO32_TMRBREG PWM12_TMRBREG
-#define DIO32_ENABLE_MASK PWM12_ENABLE_MASK
-#define DIO32_MODE PWM12_MODE
-#define DIO32_PRESCALLER PWM12_PRESCALLER
-#endif</v>
-      </c>
-      <c r="I35" s="3" t="str">
-        <f t="shared" si="5"/>
         <v>#ifdef PWM12
 mcu_config_pwm(PWM12);
 #endif</v>
@@ -39971,36 +40365,60 @@
       <c r="F36" s="6"/>
       <c r="G36" s="6"/>
       <c r="H36" s="6" t="str">
+        <f t="shared" si="5"/>
+        <v>#ifdef PWM13
+#define PWM13_CLKCTRL gclk_clkctrl(PWM13_TIMER)
+#define PWM13_PMUX (pinmux(PWM13_PORT, PWM13_BIT))
+#define PWM13_PMUXVAL (pinmuxval(PWM13_MUX))
+#if (PWM13_TIMER &lt; 3)
+#define PWM13_TMR __helper__(TCC, PWM13_TIMER, )
+#define PWM13_CONFIG (                         \
+	{                                         \
+		PWM13_TMR-&gt;CTRLA.bit.SWRST = 1;        \
+		while (PWM13_TMR-&gt;SYNCBUSY.bit.SWRST)  \
+			;                                 \
+		PWM13_TMR-&gt;CTRLA.bit.PRESCALER = 7;    \
+		PWM13_TMR-&gt;WAVE.bit.WAVEGEN = 2;       \
+		while (PWM13_TMR-&gt;SYNCBUSY.bit.WAVE)   \
+			;                                 \
+		PWM13_TMR-&gt;PER.bit.PER = 255;          \
+		while (PWM13_TMR-&gt;SYNCBUSY.bit.PER)    \
+			;                                 \
+		PWM13_TMR-&gt;CTRLA.bit.ENABLE = 1;       \
+		while (PWM13_TMR-&gt;SYNCBUSY.bit.ENABLE) \
+			;                                 \
+	})
+#define PWM13_DUTYCYCLE (PWM13_TMR-&gt;CC[PWM13_CHANNEL].bit.CC)
+#else
+#define PWM13_TMR __helper__(TC, PWM13_TIMER, )
+#define PWM13_CONFIG (                                \
+	{                                                \
+		PWM13_TMR-&gt;COUNT8.CTRLA.bit.SWRST = 1;        \
+		while (PWM13_TMR-&gt;COUNT8.STATUS.bit.SYNCBUSY) \
+			;                                        \
+		PWM13_TMR-&gt;COUNT8.CTRLA.bit.MODE = 1;         \
+		PWM13_TMR-&gt;COUNT8.CTRLA.bit.PRESCALER = 7;    \
+		PWM13_TMR-&gt;COUNT8.CTRLA.bit.WAVEGEN = 2;      \
+		while (PWM13_TMR-&gt;COUNT8.STATUS.bit.SYNCBUSY) \
+			;                                        \
+		PWM13_TMR-&gt;COUNT8.PER.reg = 255;              \
+		while (PWM13_TMR-&gt;COUNT8.STATUS.bit.SYNCBUSY) \
+			;                                        \
+		PWM13_TMR-&gt;COUNT8.CTRLA.bit.ENABLE = 1;       \
+		while (PWM13_TMR-&gt;COUNT8.STATUS.bit.SYNCBUSY) \
+			;                                        \
+	})
+#define PWM13_DUTYCYCLE (PWM13_TMR-&gt;COUNT8.CC[PWM13_CHANNEL].reg)
+#endif
+#define DIO33_PMUX PWM13_PMUX
+#define DIO33_PMUXVAL PWM13_PMUXVAL
+#define DIO33_TMR PWM13_TMR
+#define DIO33_CONFIG PWM13_CONFIG
+#define DIO33_DUTYCYCLE PWM13_DUTYCYCLE
+#endif</v>
+      </c>
+      <c r="I36" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>#if (defined(PWM13_OCR) &amp;&amp; defined(PWM13_TIMER) &amp;&amp; defined(PWM13))
-#define PWM13_OCRREG (__ocrreg__(PWM13_TIMER, PWM13_OCR))
-#define PWM13_TMRAREG (__tmrareg__(PWM13_TIMER))
-#define PWM13_TMRBREG (__tmrbreg__(PWM13_TIMER))
-#define PWM13_ENABLE_MASK __pwmenmask__(PWM13_OCR)
-#if (PWM13_TIMER == 2)
-#define PWM13_PRESCALLER 0x04
-#elif (PWM13_TIMER == 0)
-#define PWM13_PRESCALLER 0x03
-#else
-#define PWM13_PRESCALLER 0x0B
-#endif
-#if (PWM13_TIMER == 0 || PWM13_TIMER == 2)
-#define PWM13_MODE 0x03
-#else
-#define PWM13_MODE 0x01
-#endif
-#define DIO33_OCR PWM13_OCR
-#define DIO33_TIMER PWM13_TIMER
-#define DIO33_OCRREG PWM13_OCRREG
-#define DIO33_TMRAREG PWM13_TMRAREG
-#define DIO33_TMRBREG PWM13_TMRBREG
-#define DIO33_ENABLE_MASK PWM13_ENABLE_MASK
-#define DIO33_MODE PWM13_MODE
-#define DIO33_PRESCALLER PWM13_PRESCALLER
-#endif</v>
-      </c>
-      <c r="I36" s="3" t="str">
-        <f t="shared" si="5"/>
         <v>#ifdef PWM13
 mcu_config_pwm(PWM13);
 #endif</v>
@@ -40038,36 +40456,60 @@
       <c r="F37" s="6"/>
       <c r="G37" s="6"/>
       <c r="H37" s="6" t="str">
+        <f t="shared" si="5"/>
+        <v>#ifdef PWM14
+#define PWM14_CLKCTRL gclk_clkctrl(PWM14_TIMER)
+#define PWM14_PMUX (pinmux(PWM14_PORT, PWM14_BIT))
+#define PWM14_PMUXVAL (pinmuxval(PWM14_MUX))
+#if (PWM14_TIMER &lt; 3)
+#define PWM14_TMR __helper__(TCC, PWM14_TIMER, )
+#define PWM14_CONFIG (                         \
+	{                                         \
+		PWM14_TMR-&gt;CTRLA.bit.SWRST = 1;        \
+		while (PWM14_TMR-&gt;SYNCBUSY.bit.SWRST)  \
+			;                                 \
+		PWM14_TMR-&gt;CTRLA.bit.PRESCALER = 7;    \
+		PWM14_TMR-&gt;WAVE.bit.WAVEGEN = 2;       \
+		while (PWM14_TMR-&gt;SYNCBUSY.bit.WAVE)   \
+			;                                 \
+		PWM14_TMR-&gt;PER.bit.PER = 255;          \
+		while (PWM14_TMR-&gt;SYNCBUSY.bit.PER)    \
+			;                                 \
+		PWM14_TMR-&gt;CTRLA.bit.ENABLE = 1;       \
+		while (PWM14_TMR-&gt;SYNCBUSY.bit.ENABLE) \
+			;                                 \
+	})
+#define PWM14_DUTYCYCLE (PWM14_TMR-&gt;CC[PWM14_CHANNEL].bit.CC)
+#else
+#define PWM14_TMR __helper__(TC, PWM14_TIMER, )
+#define PWM14_CONFIG (                                \
+	{                                                \
+		PWM14_TMR-&gt;COUNT8.CTRLA.bit.SWRST = 1;        \
+		while (PWM14_TMR-&gt;COUNT8.STATUS.bit.SYNCBUSY) \
+			;                                        \
+		PWM14_TMR-&gt;COUNT8.CTRLA.bit.MODE = 1;         \
+		PWM14_TMR-&gt;COUNT8.CTRLA.bit.PRESCALER = 7;    \
+		PWM14_TMR-&gt;COUNT8.CTRLA.bit.WAVEGEN = 2;      \
+		while (PWM14_TMR-&gt;COUNT8.STATUS.bit.SYNCBUSY) \
+			;                                        \
+		PWM14_TMR-&gt;COUNT8.PER.reg = 255;              \
+		while (PWM14_TMR-&gt;COUNT8.STATUS.bit.SYNCBUSY) \
+			;                                        \
+		PWM14_TMR-&gt;COUNT8.CTRLA.bit.ENABLE = 1;       \
+		while (PWM14_TMR-&gt;COUNT8.STATUS.bit.SYNCBUSY) \
+			;                                        \
+	})
+#define PWM14_DUTYCYCLE (PWM14_TMR-&gt;COUNT8.CC[PWM14_CHANNEL].reg)
+#endif
+#define DIO34_PMUX PWM14_PMUX
+#define DIO34_PMUXVAL PWM14_PMUXVAL
+#define DIO34_TMR PWM14_TMR
+#define DIO34_CONFIG PWM14_CONFIG
+#define DIO34_DUTYCYCLE PWM14_DUTYCYCLE
+#endif</v>
+      </c>
+      <c r="I37" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>#if (defined(PWM14_OCR) &amp;&amp; defined(PWM14_TIMER) &amp;&amp; defined(PWM14))
-#define PWM14_OCRREG (__ocrreg__(PWM14_TIMER, PWM14_OCR))
-#define PWM14_TMRAREG (__tmrareg__(PWM14_TIMER))
-#define PWM14_TMRBREG (__tmrbreg__(PWM14_TIMER))
-#define PWM14_ENABLE_MASK __pwmenmask__(PWM14_OCR)
-#if (PWM14_TIMER == 2)
-#define PWM14_PRESCALLER 0x04
-#elif (PWM14_TIMER == 0)
-#define PWM14_PRESCALLER 0x03
-#else
-#define PWM14_PRESCALLER 0x0B
-#endif
-#if (PWM14_TIMER == 0 || PWM14_TIMER == 2)
-#define PWM14_MODE 0x03
-#else
-#define PWM14_MODE 0x01
-#endif
-#define DIO34_OCR PWM14_OCR
-#define DIO34_TIMER PWM14_TIMER
-#define DIO34_OCRREG PWM14_OCRREG
-#define DIO34_TMRAREG PWM14_TMRAREG
-#define DIO34_TMRBREG PWM14_TMRBREG
-#define DIO34_ENABLE_MASK PWM14_ENABLE_MASK
-#define DIO34_MODE PWM14_MODE
-#define DIO34_PRESCALLER PWM14_PRESCALLER
-#endif</v>
-      </c>
-      <c r="I37" s="3" t="str">
-        <f t="shared" si="5"/>
         <v>#ifdef PWM14
 mcu_config_pwm(PWM14);
 #endif</v>
@@ -40105,36 +40547,60 @@
       <c r="F38" s="6"/>
       <c r="G38" s="6"/>
       <c r="H38" s="6" t="str">
+        <f t="shared" si="5"/>
+        <v>#ifdef PWM15
+#define PWM15_CLKCTRL gclk_clkctrl(PWM15_TIMER)
+#define PWM15_PMUX (pinmux(PWM15_PORT, PWM15_BIT))
+#define PWM15_PMUXVAL (pinmuxval(PWM15_MUX))
+#if (PWM15_TIMER &lt; 3)
+#define PWM15_TMR __helper__(TCC, PWM15_TIMER, )
+#define PWM15_CONFIG (                         \
+	{                                         \
+		PWM15_TMR-&gt;CTRLA.bit.SWRST = 1;        \
+		while (PWM15_TMR-&gt;SYNCBUSY.bit.SWRST)  \
+			;                                 \
+		PWM15_TMR-&gt;CTRLA.bit.PRESCALER = 7;    \
+		PWM15_TMR-&gt;WAVE.bit.WAVEGEN = 2;       \
+		while (PWM15_TMR-&gt;SYNCBUSY.bit.WAVE)   \
+			;                                 \
+		PWM15_TMR-&gt;PER.bit.PER = 255;          \
+		while (PWM15_TMR-&gt;SYNCBUSY.bit.PER)    \
+			;                                 \
+		PWM15_TMR-&gt;CTRLA.bit.ENABLE = 1;       \
+		while (PWM15_TMR-&gt;SYNCBUSY.bit.ENABLE) \
+			;                                 \
+	})
+#define PWM15_DUTYCYCLE (PWM15_TMR-&gt;CC[PWM15_CHANNEL].bit.CC)
+#else
+#define PWM15_TMR __helper__(TC, PWM15_TIMER, )
+#define PWM15_CONFIG (                                \
+	{                                                \
+		PWM15_TMR-&gt;COUNT8.CTRLA.bit.SWRST = 1;        \
+		while (PWM15_TMR-&gt;COUNT8.STATUS.bit.SYNCBUSY) \
+			;                                        \
+		PWM15_TMR-&gt;COUNT8.CTRLA.bit.MODE = 1;         \
+		PWM15_TMR-&gt;COUNT8.CTRLA.bit.PRESCALER = 7;    \
+		PWM15_TMR-&gt;COUNT8.CTRLA.bit.WAVEGEN = 2;      \
+		while (PWM15_TMR-&gt;COUNT8.STATUS.bit.SYNCBUSY) \
+			;                                        \
+		PWM15_TMR-&gt;COUNT8.PER.reg = 255;              \
+		while (PWM15_TMR-&gt;COUNT8.STATUS.bit.SYNCBUSY) \
+			;                                        \
+		PWM15_TMR-&gt;COUNT8.CTRLA.bit.ENABLE = 1;       \
+		while (PWM15_TMR-&gt;COUNT8.STATUS.bit.SYNCBUSY) \
+			;                                        \
+	})
+#define PWM15_DUTYCYCLE (PWM15_TMR-&gt;COUNT8.CC[PWM15_CHANNEL].reg)
+#endif
+#define DIO35_PMUX PWM15_PMUX
+#define DIO35_PMUXVAL PWM15_PMUXVAL
+#define DIO35_TMR PWM15_TMR
+#define DIO35_CONFIG PWM15_CONFIG
+#define DIO35_DUTYCYCLE PWM15_DUTYCYCLE
+#endif</v>
+      </c>
+      <c r="I38" s="3" t="str">
         <f t="shared" si="4"/>
-        <v>#if (defined(PWM15_OCR) &amp;&amp; defined(PWM15_TIMER) &amp;&amp; defined(PWM15))
-#define PWM15_OCRREG (__ocrreg__(PWM15_TIMER, PWM15_OCR))
-#define PWM15_TMRAREG (__tmrareg__(PWM15_TIMER))
-#define PWM15_TMRBREG (__tmrbreg__(PWM15_TIMER))
-#define PWM15_ENABLE_MASK __pwmenmask__(PWM15_OCR)
-#if (PWM15_TIMER == 2)
-#define PWM15_PRESCALLER 0x04
-#elif (PWM15_TIMER == 0)
-#define PWM15_PRESCALLER 0x03
-#else
-#define PWM15_PRESCALLER 0x0B
-#endif
-#if (PWM15_TIMER == 0 || PWM15_TIMER == 2)
-#define PWM15_MODE 0x03
-#else
-#define PWM15_MODE 0x01
-#endif
-#define DIO35_OCR PWM15_OCR
-#define DIO35_TIMER PWM15_TIMER
-#define DIO35_OCRREG PWM15_OCRREG
-#define DIO35_TMRAREG PWM15_TMRAREG
-#define DIO35_TMRBREG PWM15_TMRBREG
-#define DIO35_ENABLE_MASK PWM15_ENABLE_MASK
-#define DIO35_MODE PWM15_MODE
-#define DIO35_PRESCALLER PWM15_PRESCALLER
-#endif</v>
-      </c>
-      <c r="I38" s="3" t="str">
-        <f t="shared" si="5"/>
         <v>#ifdef PWM15
 mcu_config_pwm(PWM15);
 #endif</v>

</xml_diff>